<commit_message>
WebApi - Added new competitions and special offer
</commit_message>
<xml_diff>
--- a/WebApi/Hattrick/BettingData/Data.xlsx
+++ b/WebApi/Hattrick/BettingData/Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UKAccounts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Hattrick-Zadatak\WebApi\Hattrick\BettingData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A570342E-6F03-4219-98DB-BC046504DB80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DC6F5AE-6F78-41A1-AD4E-DEF7ADAEDD31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8A8FB8C8-DECA-43B5-BE20-421A0553B977}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="66">
   <si>
     <t>Use ICNID34508</t>
   </si>
@@ -90,9 +90,6 @@
     <t>MatchId</t>
   </si>
   <si>
-    <t>4.11. 18:00</t>
-  </si>
-  <si>
     <t>Sl.Belupo</t>
   </si>
   <si>
@@ -105,9 +102,6 @@
     <t>Osijek</t>
   </si>
   <si>
-    <t>5.11. 17:30</t>
-  </si>
-  <si>
     <t>NK Varaždin</t>
   </si>
   <si>
@@ -135,9 +129,6 @@
     <t>Brighton</t>
   </si>
   <si>
-    <t>5.11. 16:00</t>
-  </si>
-  <si>
     <t>Leeds</t>
   </si>
   <si>
@@ -160,6 +151,90 @@
   </si>
   <si>
     <t>Leicester</t>
+  </si>
+  <si>
+    <t>Španjolska 1</t>
+  </si>
+  <si>
+    <t>Espanyol</t>
+  </si>
+  <si>
+    <t>Villarreal</t>
+  </si>
+  <si>
+    <t>Real Madrid</t>
+  </si>
+  <si>
+    <t>Cadiz</t>
+  </si>
+  <si>
+    <t>10.11. 20:30</t>
+  </si>
+  <si>
+    <t>Atl. Madrid</t>
+  </si>
+  <si>
+    <t>Elche</t>
+  </si>
+  <si>
+    <t>10.11. 20:00</t>
+  </si>
+  <si>
+    <t>Valencia</t>
+  </si>
+  <si>
+    <t>Betis</t>
+  </si>
+  <si>
+    <t>Italija 1</t>
+  </si>
+  <si>
+    <t>Fiorentina</t>
+  </si>
+  <si>
+    <t>Salernitana</t>
+  </si>
+  <si>
+    <t>Inter M.</t>
+  </si>
+  <si>
+    <t>Bologna</t>
+  </si>
+  <si>
+    <t>09.11. 20:45</t>
+  </si>
+  <si>
+    <t>09.11. 20:00</t>
+  </si>
+  <si>
+    <t>05.11. 16:00</t>
+  </si>
+  <si>
+    <t>05.11. 17:30</t>
+  </si>
+  <si>
+    <t>04.11. 18:00</t>
+  </si>
+  <si>
+    <t>H.Verona</t>
+  </si>
+  <si>
+    <t>Juventus</t>
+  </si>
+  <si>
+    <t>Lazio</t>
+  </si>
+  <si>
+    <t>Monza</t>
+  </si>
+  <si>
+    <t>Lecce</t>
+  </si>
+  <si>
+    <t>13.11. 20:45</t>
+  </si>
+  <si>
+    <t>Sampdoria</t>
   </si>
 </sst>
 </file>
@@ -621,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A6D1DB7-EB0F-4CE0-A63D-2F8F461E49B4}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -712,10 +787,10 @@
         <v>1.45</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="L2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -726,10 +801,10 @@
         <v>15</v>
       </c>
       <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
         <v>18</v>
-      </c>
-      <c r="D3" t="s">
-        <v>19</v>
       </c>
       <c r="E3" s="3">
         <v>2.7</v>
@@ -750,7 +825,7 @@
         <v>1.3</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="L3" t="b">
         <v>0</v>
@@ -764,10 +839,10 @@
         <v>15</v>
       </c>
       <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
         <v>20</v>
-      </c>
-      <c r="D4" t="s">
-        <v>21</v>
       </c>
       <c r="E4" s="3">
         <v>1.85</v>
@@ -788,10 +863,10 @@
         <v>1.27</v>
       </c>
       <c r="K4" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="L4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -802,10 +877,10 @@
         <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E5" s="3">
         <v>2.4</v>
@@ -826,7 +901,7 @@
         <v>1.3</v>
       </c>
       <c r="K5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="L5" t="b">
         <v>0</v>
@@ -840,10 +915,10 @@
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E6" s="3">
         <v>1.2</v>
@@ -864,10 +939,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="K6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="L6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -875,13 +950,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
         <v>29</v>
-      </c>
-      <c r="C7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" t="s">
-        <v>31</v>
       </c>
       <c r="E7" s="3">
         <v>3.4</v>
@@ -902,10 +977,10 @@
         <v>1.35</v>
       </c>
       <c r="K7" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="L7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -913,13 +988,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E8" s="3">
         <v>1.75</v>
@@ -940,10 +1015,10 @@
         <v>1.3</v>
       </c>
       <c r="K8" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="L8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -951,13 +1026,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E9" s="3">
         <v>2.75</v>
@@ -978,10 +1053,10 @@
         <v>1.35</v>
       </c>
       <c r="K9" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="L9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -989,13 +1064,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E10" s="3">
         <v>1.1499999999999999</v>
@@ -1016,10 +1091,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="K10" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="L10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -1027,13 +1102,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E11" s="3">
         <v>2.4500000000000002</v>
@@ -1054,9 +1129,351 @@
         <v>1.35</v>
       </c>
       <c r="K11" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="L11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="3">
+        <v>2.85</v>
+      </c>
+      <c r="F12" s="3">
+        <v>3.3</v>
+      </c>
+      <c r="G12" s="3">
+        <v>2.6</v>
+      </c>
+      <c r="H12" s="3">
+        <v>1.55</v>
+      </c>
+      <c r="I12" s="3">
+        <v>1.45</v>
+      </c>
+      <c r="J12" s="3">
+        <v>1.35</v>
+      </c>
+      <c r="K12" t="s">
+        <v>55</v>
+      </c>
+      <c r="L12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="3">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="F13" s="3">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="G13" s="3">
+        <v>17</v>
+      </c>
+      <c r="H13" s="3">
+        <v>1.02</v>
+      </c>
+      <c r="I13" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="J13" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K13" t="s">
+        <v>43</v>
+      </c>
+      <c r="L13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1.3</v>
+      </c>
+      <c r="F14" s="3">
+        <v>5.6</v>
+      </c>
+      <c r="G14" s="3">
+        <v>10</v>
+      </c>
+      <c r="H14" s="3">
+        <v>1.05</v>
+      </c>
+      <c r="I14" s="3">
+        <v>3.6</v>
+      </c>
+      <c r="J14" s="3">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="K14" t="s">
+        <v>46</v>
+      </c>
+      <c r="L14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F15" s="3">
+        <v>3.4</v>
+      </c>
+      <c r="G15" s="3">
+        <v>3.4</v>
+      </c>
+      <c r="H15" s="3">
+        <v>1.35</v>
+      </c>
+      <c r="I15" s="3">
+        <v>1.7</v>
+      </c>
+      <c r="J15" s="3">
+        <v>1.35</v>
+      </c>
+      <c r="K15" t="s">
+        <v>43</v>
+      </c>
+      <c r="L15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="3">
+        <v>1.55</v>
+      </c>
+      <c r="F16" s="3">
+        <v>4.3</v>
+      </c>
+      <c r="G16" s="3">
+        <v>6</v>
+      </c>
+      <c r="H16" s="3">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="I16" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="J16" s="3">
+        <v>1.25</v>
+      </c>
+      <c r="K16" t="s">
+        <v>54</v>
+      </c>
+      <c r="L16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="F17" s="3">
+        <v>5.2</v>
+      </c>
+      <c r="G17" s="3">
+        <v>7.6</v>
+      </c>
+      <c r="H17" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I17" s="3">
+        <v>3.1</v>
+      </c>
+      <c r="J17" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="K17" t="s">
+        <v>54</v>
+      </c>
+      <c r="L17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="3">
+        <v>5</v>
+      </c>
+      <c r="F18" s="3">
+        <v>3.8</v>
+      </c>
+      <c r="G18" s="3">
+        <v>1.75</v>
+      </c>
+      <c r="H18" s="3">
+        <v>2.15</v>
+      </c>
+      <c r="I18" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="J18" s="3">
+        <v>1.3</v>
+      </c>
+      <c r="K18" t="s">
+        <v>54</v>
+      </c>
+      <c r="L18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19" s="3">
+        <v>1.65</v>
+      </c>
+      <c r="F19" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="G19" s="3">
+        <v>5</v>
+      </c>
+      <c r="H19" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="I19" s="3">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="J19" s="3">
+        <v>1.25</v>
+      </c>
+      <c r="K19" t="s">
+        <v>54</v>
+      </c>
+      <c r="L19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" s="3">
+        <v>2.6</v>
+      </c>
+      <c r="F20" s="3">
+        <v>3.1</v>
+      </c>
+      <c r="G20" s="3">
+        <v>2.95</v>
+      </c>
+      <c r="H20" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="I20" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="J20" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="K20" t="s">
+        <v>64</v>
+      </c>
+      <c r="L20" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
WebApi - Add nullable bet fields
</commit_message>
<xml_diff>
--- a/WebApi/Hattrick/BettingData/Data.xlsx
+++ b/WebApi/Hattrick/BettingData/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Hattrick-Zadatak\WebApi\Hattrick\BettingData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DC6F5AE-6F78-41A1-AD4E-DEF7ADAEDD31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C14485C7-18A0-487B-8DE0-E88D2865F5D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8A8FB8C8-DECA-43B5-BE20-421A0553B977}"/>
   </bookViews>
@@ -699,7 +699,7 @@
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -929,9 +929,7 @@
       <c r="G6" s="3">
         <v>14</v>
       </c>
-      <c r="H6" s="3">
-        <v>1.01</v>
-      </c>
+      <c r="H6" s="3"/>
       <c r="I6" s="3">
         <v>4.2</v>
       </c>

</xml_diff>

<commit_message>
WebApi - Added basketball and tennis APIs, added new matches to Data file
</commit_message>
<xml_diff>
--- a/WebApi/Hattrick/BettingData/Data.xlsx
+++ b/WebApi/Hattrick/BettingData/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Hattrick-Zadatak\WebApi\Hattrick\BettingData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C14485C7-18A0-487B-8DE0-E88D2865F5D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4421A5FF-5A38-492A-9DA3-FB44071F1616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8A8FB8C8-DECA-43B5-BE20-421A0553B977}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="116">
   <si>
     <t>Use ICNID34508</t>
   </si>
@@ -235,6 +235,156 @@
   </si>
   <si>
     <t>Sampdoria</t>
+  </si>
+  <si>
+    <t>NBA</t>
+  </si>
+  <si>
+    <t>Charlotte Hornets</t>
+  </si>
+  <si>
+    <t>Indiana Pacers</t>
+  </si>
+  <si>
+    <t>Orlando Magic</t>
+  </si>
+  <si>
+    <t>Minnesota Timberw.</t>
+  </si>
+  <si>
+    <t>Toronto Raptors</t>
+  </si>
+  <si>
+    <t>Dallas Mavericks</t>
+  </si>
+  <si>
+    <t>Houston Rockets</t>
+  </si>
+  <si>
+    <t>Denver Nuggets</t>
+  </si>
+  <si>
+    <t>Miami Heat</t>
+  </si>
+  <si>
+    <t>New York Knicks</t>
+  </si>
+  <si>
+    <t>Phoenix Suns</t>
+  </si>
+  <si>
+    <t>Golden State W.</t>
+  </si>
+  <si>
+    <t>13.11. 01:00</t>
+  </si>
+  <si>
+    <t>13.11. 04:00</t>
+  </si>
+  <si>
+    <t>13.11. 02:30</t>
+  </si>
+  <si>
+    <t>Euroleague</t>
+  </si>
+  <si>
+    <t>Anadolu Efes</t>
+  </si>
+  <si>
+    <t>Barcelona Lassa</t>
+  </si>
+  <si>
+    <t>CZ Beograd</t>
+  </si>
+  <si>
+    <t>ASVEL Lyon</t>
+  </si>
+  <si>
+    <t>Bayern Munchen</t>
+  </si>
+  <si>
+    <t>Olympiacos BC</t>
+  </si>
+  <si>
+    <t>Virtus Bologna</t>
+  </si>
+  <si>
+    <t>Valencia BC</t>
+  </si>
+  <si>
+    <t>ALBA Berlin</t>
+  </si>
+  <si>
+    <t>13.11. 20:30</t>
+  </si>
+  <si>
+    <t>13.11. 19:00</t>
+  </si>
+  <si>
+    <t>Wimbledon</t>
+  </si>
+  <si>
+    <t>Đoković N</t>
+  </si>
+  <si>
+    <t>Sinner J.</t>
+  </si>
+  <si>
+    <t>Fritz T.</t>
+  </si>
+  <si>
+    <t>Nadal R.</t>
+  </si>
+  <si>
+    <t>Goffin D.</t>
+  </si>
+  <si>
+    <t>Norrie C</t>
+  </si>
+  <si>
+    <t>Garin C.</t>
+  </si>
+  <si>
+    <t>Kyrgios N.</t>
+  </si>
+  <si>
+    <t>13.11. 13:45</t>
+  </si>
+  <si>
+    <t>13.11. 16:00</t>
+  </si>
+  <si>
+    <t>ATP Umag</t>
+  </si>
+  <si>
+    <t>Alcaraz C.</t>
+  </si>
+  <si>
+    <t>Bagnis F.</t>
+  </si>
+  <si>
+    <t>Zapata Miralles B.</t>
+  </si>
+  <si>
+    <t>Zeppieri G.</t>
+  </si>
+  <si>
+    <t>Carballes Baena R.</t>
+  </si>
+  <si>
+    <t>Gombos N.</t>
+  </si>
+  <si>
+    <t>Cecchinato M.</t>
+  </si>
+  <si>
+    <t>Agamenone F.</t>
+  </si>
+  <si>
+    <t>13.11. 17:00</t>
+  </si>
+  <si>
+    <t>13.11. 20:00</t>
   </si>
 </sst>
 </file>
@@ -696,10 +846,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A6D1DB7-EB0F-4CE0-A63D-2F8F461E49B4}">
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="L39" sqref="L39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1475,6 +1625,599 @@
         <v>0</v>
       </c>
     </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21" s="3">
+        <v>1.75</v>
+      </c>
+      <c r="F21" s="3">
+        <v>13</v>
+      </c>
+      <c r="G21" s="3">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="H21" s="3">
+        <v>1.55</v>
+      </c>
+      <c r="I21" s="3">
+        <v>2</v>
+      </c>
+      <c r="K21" t="s">
+        <v>79</v>
+      </c>
+      <c r="L21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" t="s">
+        <v>70</v>
+      </c>
+      <c r="E22" s="3">
+        <v>2.9</v>
+      </c>
+      <c r="F22" s="3">
+        <v>15</v>
+      </c>
+      <c r="G22" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="H22" s="3">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="I22" s="3">
+        <v>1.35</v>
+      </c>
+      <c r="K22" t="s">
+        <v>79</v>
+      </c>
+      <c r="L22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" t="s">
+        <v>75</v>
+      </c>
+      <c r="E23" s="3">
+        <v>2.1</v>
+      </c>
+      <c r="F23" s="3">
+        <v>13</v>
+      </c>
+      <c r="G23" s="3">
+        <v>1.85</v>
+      </c>
+      <c r="H23" s="3">
+        <v>1.8</v>
+      </c>
+      <c r="I23" s="3">
+        <v>1.65</v>
+      </c>
+      <c r="K23" t="s">
+        <v>81</v>
+      </c>
+      <c r="L23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" t="s">
+        <v>72</v>
+      </c>
+      <c r="D24" t="s">
+        <v>73</v>
+      </c>
+      <c r="E24" s="3">
+        <v>1.25</v>
+      </c>
+      <c r="F24" s="3">
+        <v>17</v>
+      </c>
+      <c r="G24" s="3">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="H24" s="3">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="I24" s="3">
+        <v>3.6</v>
+      </c>
+      <c r="K24" t="s">
+        <v>81</v>
+      </c>
+      <c r="L24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25" t="s">
+        <v>76</v>
+      </c>
+      <c r="E25" s="3">
+        <v>1.65</v>
+      </c>
+      <c r="F25" s="3">
+        <v>14</v>
+      </c>
+      <c r="G25" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="H25" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="I25" s="3">
+        <v>2.1</v>
+      </c>
+      <c r="K25" t="s">
+        <v>80</v>
+      </c>
+      <c r="L25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" t="s">
+        <v>77</v>
+      </c>
+      <c r="D26" t="s">
+        <v>78</v>
+      </c>
+      <c r="E26" s="3">
+        <v>2</v>
+      </c>
+      <c r="F26" s="3">
+        <v>15</v>
+      </c>
+      <c r="G26" s="3">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="H26" s="3">
+        <v>1.8</v>
+      </c>
+      <c r="I26" s="3">
+        <v>2</v>
+      </c>
+      <c r="K26" t="s">
+        <v>80</v>
+      </c>
+      <c r="L26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>82</v>
+      </c>
+      <c r="C27" t="s">
+        <v>83</v>
+      </c>
+      <c r="D27" t="s">
+        <v>84</v>
+      </c>
+      <c r="E27" s="3">
+        <v>1.85</v>
+      </c>
+      <c r="F27" s="3">
+        <v>13</v>
+      </c>
+      <c r="G27" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H27" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="I27" s="3">
+        <v>1.85</v>
+      </c>
+      <c r="K27" t="s">
+        <v>93</v>
+      </c>
+      <c r="L27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>82</v>
+      </c>
+      <c r="C28" t="s">
+        <v>85</v>
+      </c>
+      <c r="D28" t="s">
+        <v>86</v>
+      </c>
+      <c r="E28" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="F28" s="3">
+        <v>15</v>
+      </c>
+      <c r="G28" s="3">
+        <v>2.9</v>
+      </c>
+      <c r="H28" s="3">
+        <v>1.35</v>
+      </c>
+      <c r="I28" s="3">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="K28" t="s">
+        <v>93</v>
+      </c>
+      <c r="L28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" t="s">
+        <v>87</v>
+      </c>
+      <c r="D29" t="s">
+        <v>88</v>
+      </c>
+      <c r="E29" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="F29" s="3">
+        <v>14</v>
+      </c>
+      <c r="G29" s="3">
+        <v>1.65</v>
+      </c>
+      <c r="H29" s="3">
+        <v>2.1</v>
+      </c>
+      <c r="I29" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="K29" t="s">
+        <v>92</v>
+      </c>
+      <c r="L29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>82</v>
+      </c>
+      <c r="C30" t="s">
+        <v>89</v>
+      </c>
+      <c r="D30" t="s">
+        <v>90</v>
+      </c>
+      <c r="E30" s="3">
+        <v>1.55</v>
+      </c>
+      <c r="F30" s="3">
+        <v>15</v>
+      </c>
+      <c r="G30" s="3">
+        <v>2.8</v>
+      </c>
+      <c r="H30" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="I30" s="3">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="K30" t="s">
+        <v>92</v>
+      </c>
+      <c r="L30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>82</v>
+      </c>
+      <c r="C31" t="s">
+        <v>41</v>
+      </c>
+      <c r="D31" t="s">
+        <v>91</v>
+      </c>
+      <c r="E31" s="3">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="F31" s="3">
+        <v>18</v>
+      </c>
+      <c r="G31" s="3">
+        <v>5.4</v>
+      </c>
+      <c r="H31" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I31" s="3">
+        <v>4.8</v>
+      </c>
+      <c r="K31" t="s">
+        <v>64</v>
+      </c>
+      <c r="L31" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" t="s">
+        <v>95</v>
+      </c>
+      <c r="D32" t="s">
+        <v>96</v>
+      </c>
+      <c r="E32" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G32" s="3">
+        <v>6.5</v>
+      </c>
+      <c r="K32" t="s">
+        <v>103</v>
+      </c>
+      <c r="L32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>94</v>
+      </c>
+      <c r="C33" t="s">
+        <v>97</v>
+      </c>
+      <c r="D33" t="s">
+        <v>98</v>
+      </c>
+      <c r="E33" s="3">
+        <v>2.75</v>
+      </c>
+      <c r="G33" s="3">
+        <v>1.45</v>
+      </c>
+      <c r="K33" t="s">
+        <v>103</v>
+      </c>
+      <c r="L33" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>94</v>
+      </c>
+      <c r="C34" t="s">
+        <v>99</v>
+      </c>
+      <c r="D34" t="s">
+        <v>100</v>
+      </c>
+      <c r="E34" s="3">
+        <v>2.9</v>
+      </c>
+      <c r="G34" s="3">
+        <v>1.3</v>
+      </c>
+      <c r="K34" t="s">
+        <v>104</v>
+      </c>
+      <c r="L34" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>94</v>
+      </c>
+      <c r="C35" t="s">
+        <v>101</v>
+      </c>
+      <c r="D35" t="s">
+        <v>102</v>
+      </c>
+      <c r="E35" s="3">
+        <v>4.3</v>
+      </c>
+      <c r="G35" s="3">
+        <v>1.25</v>
+      </c>
+      <c r="K35" t="s">
+        <v>104</v>
+      </c>
+      <c r="L35" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>105</v>
+      </c>
+      <c r="C36" t="s">
+        <v>106</v>
+      </c>
+      <c r="D36" t="s">
+        <v>107</v>
+      </c>
+      <c r="E36" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G36" s="3">
+        <v>9</v>
+      </c>
+      <c r="K36" t="s">
+        <v>114</v>
+      </c>
+      <c r="L36" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>105</v>
+      </c>
+      <c r="C37" t="s">
+        <v>108</v>
+      </c>
+      <c r="D37" t="s">
+        <v>109</v>
+      </c>
+      <c r="E37" s="3">
+        <v>1.55</v>
+      </c>
+      <c r="G37" s="3">
+        <v>2.4</v>
+      </c>
+      <c r="K37" t="s">
+        <v>114</v>
+      </c>
+      <c r="L37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>105</v>
+      </c>
+      <c r="C38" t="s">
+        <v>110</v>
+      </c>
+      <c r="D38" t="s">
+        <v>111</v>
+      </c>
+      <c r="E38" s="3">
+        <v>5</v>
+      </c>
+      <c r="G38" s="3">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="K38" t="s">
+        <v>115</v>
+      </c>
+      <c r="L38" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>105</v>
+      </c>
+      <c r="C39" t="s">
+        <v>112</v>
+      </c>
+      <c r="D39" t="s">
+        <v>113</v>
+      </c>
+      <c r="E39" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="G39" s="3">
+        <v>2.4</v>
+      </c>
+      <c r="K39" t="s">
+        <v>115</v>
+      </c>
+      <c r="L39" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
WebApi - Add match outcome
</commit_message>
<xml_diff>
--- a/WebApi/Hattrick/BettingData/Data.xlsx
+++ b/WebApi/Hattrick/BettingData/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Hattrick-Zadatak\WebApi\Hattrick\BettingData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4421A5FF-5A38-492A-9DA3-FB44071F1616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDEA1E17-FB73-45D0-AC2B-5CD1F6EDCC4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8A8FB8C8-DECA-43B5-BE20-421A0553B977}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="120">
   <si>
     <t>Use ICNID34508</t>
   </si>
@@ -385,6 +385,18 @@
   </si>
   <si>
     <t>13.11. 20:00</t>
+  </si>
+  <si>
+    <t>MatchOutcome</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
 </sst>
 </file>
@@ -432,12 +444,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -846,10 +859,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A6D1DB7-EB0F-4CE0-A63D-2F8F461E49B4}">
-  <dimension ref="A1:L39"/>
+  <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="L39" sqref="L39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -865,9 +878,10 @@
     <col min="10" max="10" width="14.140625" customWidth="1"/>
     <col min="11" max="11" width="17.140625" customWidth="1"/>
     <col min="12" max="12" width="13.140625" customWidth="1"/>
+    <col min="13" max="13" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -904,8 +918,11 @@
       <c r="L1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -942,8 +959,11 @@
       <c r="L2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -980,8 +1000,11 @@
       <c r="L3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1018,8 +1041,11 @@
       <c r="L4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1056,8 +1082,11 @@
       <c r="L5" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M5" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1092,8 +1121,11 @@
       <c r="L6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1130,8 +1162,9 @@
       <c r="L7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M7" s="5"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1168,8 +1201,9 @@
       <c r="L8" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M8" s="5"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1206,8 +1240,9 @@
       <c r="L9" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M9" s="5"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1244,8 +1279,11 @@
       <c r="L10" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M10" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1282,8 +1320,9 @@
       <c r="L11" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M11" s="5"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1320,8 +1359,9 @@
       <c r="L12" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M12" s="5"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1358,8 +1398,11 @@
       <c r="L13" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M13" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1396,8 +1439,11 @@
       <c r="L14" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M14" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1434,8 +1480,9 @@
       <c r="L15" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M15" s="5"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1472,8 +1519,9 @@
       <c r="L16" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M16" s="5"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1510,8 +1558,9 @@
       <c r="L17" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M17" s="5"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1548,8 +1597,11 @@
       <c r="L18" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M18" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1586,8 +1638,9 @@
       <c r="L19" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M19" s="5"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1624,8 +1677,9 @@
       <c r="L20" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M20" s="5"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1659,8 +1713,9 @@
       <c r="L21" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M21" s="5"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1694,8 +1749,9 @@
       <c r="L22" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M22" s="5"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1729,8 +1785,9 @@
       <c r="L23" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M23" s="5"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1764,8 +1821,9 @@
       <c r="L24" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M24" s="5"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1799,8 +1857,9 @@
       <c r="L25" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M25" s="5"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1834,8 +1893,9 @@
       <c r="L26" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M26" s="5"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1869,8 +1929,9 @@
       <c r="L27" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M27" s="5"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1904,8 +1965,9 @@
       <c r="L28" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M28" s="5"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1939,8 +2001,9 @@
       <c r="L29" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M29" s="5"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1974,8 +2037,9 @@
       <c r="L30" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M30" s="5"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2009,8 +2073,9 @@
       <c r="L31" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M31" s="5"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2035,8 +2100,9 @@
       <c r="L32" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M32" s="5"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2061,8 +2127,9 @@
       <c r="L33" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M33" s="5"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2087,8 +2154,9 @@
       <c r="L34" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M34" s="5"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2113,8 +2181,9 @@
       <c r="L35" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M35" s="5"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2139,8 +2208,9 @@
       <c r="L36" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M36" s="5"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2165,8 +2235,9 @@
       <c r="L37" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M37" s="5"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2191,8 +2262,9 @@
       <c r="L38" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M38" s="5"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2217,6 +2289,7 @@
       <c r="L39" t="b">
         <v>0</v>
       </c>
+      <c r="M39" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
WebApi - Create MatchOutcome API, code styling
</commit_message>
<xml_diff>
--- a/WebApi/Hattrick/BettingData/Data.xlsx
+++ b/WebApi/Hattrick/BettingData/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Hattrick-Zadatak\WebApi\Hattrick\BettingData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDEA1E17-FB73-45D0-AC2B-5CD1F6EDCC4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{072C689C-A40A-4B79-A9C9-820F61174334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8A8FB8C8-DECA-43B5-BE20-421A0553B977}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="117">
   <si>
     <t>Use ICNID34508</t>
   </si>
@@ -388,15 +388,6 @@
   </si>
   <si>
     <t>MatchOutcome</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
   </si>
 </sst>
 </file>
@@ -862,7 +853,7 @@
   <dimension ref="A1:M39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -959,9 +950,7 @@
       <c r="L2" t="b">
         <v>1</v>
       </c>
-      <c r="M2" s="5" t="s">
-        <v>119</v>
-      </c>
+      <c r="M2" s="5"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -1000,9 +989,7 @@
       <c r="L3" t="b">
         <v>0</v>
       </c>
-      <c r="M3" s="5" t="s">
-        <v>118</v>
-      </c>
+      <c r="M3" s="5"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -1041,9 +1028,7 @@
       <c r="L4" t="b">
         <v>1</v>
       </c>
-      <c r="M4" s="5" t="s">
-        <v>118</v>
-      </c>
+      <c r="M4" s="5"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -1082,9 +1067,7 @@
       <c r="L5" t="b">
         <v>0</v>
       </c>
-      <c r="M5" s="5" t="s">
-        <v>119</v>
-      </c>
+      <c r="M5" s="5"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -1121,9 +1104,7 @@
       <c r="L6" t="b">
         <v>1</v>
       </c>
-      <c r="M6" s="5" t="s">
-        <v>117</v>
-      </c>
+      <c r="M6" s="5"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -1279,9 +1260,7 @@
       <c r="L10" t="b">
         <v>1</v>
       </c>
-      <c r="M10" s="5" t="s">
-        <v>118</v>
-      </c>
+      <c r="M10" s="5"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -1398,9 +1377,7 @@
       <c r="L13" t="b">
         <v>0</v>
       </c>
-      <c r="M13" s="5" t="s">
-        <v>118</v>
-      </c>
+      <c r="M13" s="5"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -1439,9 +1416,7 @@
       <c r="L14" t="b">
         <v>1</v>
       </c>
-      <c r="M14" s="5" t="s">
-        <v>117</v>
-      </c>
+      <c r="M14" s="5"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -1597,9 +1572,7 @@
       <c r="L18" t="b">
         <v>1</v>
       </c>
-      <c r="M18" s="5" t="s">
-        <v>117</v>
-      </c>
+      <c r="M18" s="5"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">

</xml_diff>